<commit_message>
addback some models, create others
</commit_message>
<xml_diff>
--- a/BMY.xlsx
+++ b/BMY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB5B77-CD91-420C-9FCB-B1640D86D7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DAEB6C-A7DE-43CC-84C3-F84FCE947FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41730" yWindow="1050" windowWidth="30405" windowHeight="18060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32130" yWindow="3510" windowWidth="30195" windowHeight="16815" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="23" r:id="rId1"/>
@@ -7289,10 +7289,10 @@
   <dimension ref="A1:FY150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="BO126" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="BO3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CB149" sqref="CB149"/>
+      <selection pane="bottomRight" activeCell="BQ15" sqref="BQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29749,27 +29749,27 @@
         <v>-45379</v>
       </c>
       <c r="CC94" s="35">
-        <f>+CB94+CC67</f>
+        <f t="shared" ref="CC94:CH94" si="341">+CB94+CC67</f>
         <v>-41487.116320000001</v>
       </c>
       <c r="CD94" s="35">
-        <f>+CC94+CD67</f>
+        <f t="shared" si="341"/>
         <v>-37357.570720000003</v>
       </c>
       <c r="CE94" s="35">
-        <f>+CD94+CE67</f>
+        <f t="shared" si="341"/>
         <v>-32733.672400000003</v>
       </c>
       <c r="CF94" s="35">
-        <f>+CE94+CF67</f>
+        <f t="shared" si="341"/>
         <v>-27823.398273600003</v>
       </c>
       <c r="CG94" s="35">
-        <f>+CF94+CG67</f>
+        <f t="shared" si="341"/>
         <v>-23307.632356800001</v>
       </c>
       <c r="CH94" s="35">
-        <f>+CG94+CH67</f>
+        <f t="shared" si="341"/>
         <v>-18644.736451199999</v>
       </c>
       <c r="CI94" s="35"/>
@@ -29819,43 +29819,43 @@
         <v>-18644.736451199999</v>
       </c>
       <c r="DW94" s="44">
-        <f>+DV94+DW67</f>
+        <f t="shared" ref="DW94:EF94" si="342">+DV94+DW67</f>
         <v>7546.0087013200027</v>
       </c>
       <c r="DX94" s="44">
-        <f>+DW94+DX67</f>
+        <f t="shared" si="342"/>
         <v>34954.279951278964</v>
       </c>
       <c r="DY94" s="44">
-        <f>+DX94+DY67</f>
+        <f t="shared" si="342"/>
         <v>60601.963702859772</v>
       </c>
       <c r="DZ94" s="44">
-        <f>+DY94+DZ67</f>
+        <f t="shared" si="342"/>
         <v>84417.176206873322</v>
       </c>
       <c r="EA94" s="44">
-        <f>+DZ94+EA67</f>
+        <f t="shared" si="342"/>
         <v>108762.44028843251</v>
       </c>
       <c r="EB94" s="44">
-        <f>+EA94+EB67</f>
+        <f t="shared" si="342"/>
         <v>133950.96366000862</v>
       </c>
       <c r="EC94" s="44">
-        <f>+EB94+EC67</f>
+        <f t="shared" si="342"/>
         <v>159862.86939798042</v>
       </c>
       <c r="ED94" s="44">
-        <f>+EC94+ED67</f>
+        <f t="shared" si="342"/>
         <v>177721.3293295858</v>
       </c>
       <c r="EE94" s="44">
-        <f>+ED94+EE67</f>
+        <f t="shared" si="342"/>
         <v>193717.63797271263</v>
       </c>
       <c r="EF94" s="44">
-        <f>+EE94+EF67</f>
+        <f t="shared" si="342"/>
         <v>203157.75166403185</v>
       </c>
     </row>
@@ -34569,18 +34569,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34698,18 +34698,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AC6227C-4700-4C6A-A399-7F39853AD9C6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2206DA00-2832-4926-9B8E-385E975B4BC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2206DA00-2832-4926-9B8E-385E975B4BC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AC6227C-4700-4C6A-A399-7F39853AD9C6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>